<commit_message>
BackgroundjobBump to MS 7.0.16Update Chat messageDone Chat Function
</commit_message>
<xml_diff>
--- a/src/Host/Output/AssetDeliceryFrom.xlsx
+++ b/src/Host/Output/AssetDeliceryFrom.xlsx
@@ -16,15 +16,15 @@
     <x:sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Assets_tpl" localSheetId="0">Sheet1!$A$22:$I$23</x:definedName>
-    <x:definedName name="Assets">Sheet1!$A$22:$I$23</x:definedName>
+    <x:definedName name="Assets_tpl" localSheetId="0">Sheet1!$A$22:$I$25</x:definedName>
+    <x:definedName name="Assets">Sheet1!$A$22:$I$25</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="191029"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t xml:space="preserve">CÔNG TY CỔ PHẦN TARA </x:t>
   </x:si>
@@ -73,13 +73,13 @@
     <x:t>Chức danh:</x:t>
   </x:si>
   <x:si>
-    <x:t>AGM</x:t>
+    <x:t xml:space="preserve">Cashier </x:t>
   </x:si>
   <x:si>
     <x:t>Mã Nhân viên:</x:t>
   </x:si>
   <x:si>
-    <x:t>21707</x:t>
+    <x:t>11260</x:t>
   </x:si>
   <x:si>
     <x:t>Phòng/ Bộ phận:</x:t>
@@ -112,25 +112,34 @@
     <x:t>Ghi chú</x:t>
   </x:si>
   <x:si>
-    <x:t>01-CC-TB-0424</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dell Latitude 3480_L3480I514DF, Intel Core i5-6200U, 4GB RAM, 500GB HDD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-CC-0640</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HP Printer Laser Jet Pro M12w</x:t>
+    <x:t>01-CC-TB-0187</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Ổ cứng di động Transcend A3 1TB </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-CC-TB-0167</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAMSUNG LCD 17”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-CC-TB-0326</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CPU Core I3 6100, 8Gb Ram, HDD 1Tb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-CC-TB-0347</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Ổ cứng di động WD Elements 2TB </x:t>
   </x:si>
   <x:si>
     <x:t>Điều 2: Trách nhiệm</x:t>
   </x:si>
   <x:si>
     <x:t>- Bên B có trách nhiệm bảo vệ trang thiết bị được giao, tránh để bị hỏng hóc do các yếu tố ngoại cảnh và không để mất mát. (ở công ty, ở nhà và trên đường đến công ty và về nhà).</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
   </x:si>
   <x:si>
     <x:t>- Bên B không được thay đổi cấu hình trang thiết bị được giao (phần cứng, phần mềm) khi không có sự đồng ý của bên A</x:t>
@@ -1006,7 +1015,7 @@
   <x:dimension ref="A2:I40"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <x:selection activeCell="B40" sqref="B40 B40:D40"/>
+      <x:selection activeCell="B40" sqref="B40 B42:D42"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1033,65 +1042,65 @@
       <x:c r="B3" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s"/>
-      <x:c r="D3" s="2" t="s"/>
-      <x:c r="E3" s="2" t="s"/>
-      <x:c r="F3" s="2" t="s"/>
-      <x:c r="G3" s="2" t="s"/>
-      <x:c r="H3" s="2" t="s"/>
-      <x:c r="I3" s="2" t="s"/>
+      <x:c r="C3" s="2"/>
+      <x:c r="D3" s="2"/>
+      <x:c r="E3" s="2"/>
+      <x:c r="F3" s="2"/>
+      <x:c r="G3" s="2"/>
+      <x:c r="H3" s="2"/>
+      <x:c r="I3" s="2"/>
     </x:row>
     <x:row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B4" s="12" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C4" s="12" t="s"/>
-      <x:c r="D4" s="12" t="s"/>
+      <x:c r="C4" s="12"/>
+      <x:c r="D4" s="12"/>
       <x:c r="E4" s="12" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="F4" s="12" t="s"/>
-      <x:c r="G4" s="12" t="s"/>
-      <x:c r="H4" s="12" t="s"/>
-      <x:c r="I4" s="12" t="s"/>
+      <x:c r="F4" s="12"/>
+      <x:c r="G4" s="12"/>
+      <x:c r="H4" s="12"/>
+      <x:c r="I4" s="12"/>
     </x:row>
     <x:row r="5" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="B5" s="34" t="s"/>
-      <x:c r="C5" s="34" t="s"/>
+      <x:c r="B5" s="34"/>
+      <x:c r="C5" s="34"/>
       <x:c r="D5" s="30" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="E5" s="31" t="s"/>
-      <x:c r="F5" s="31" t="s"/>
-      <x:c r="G5" s="31" t="s"/>
+      <x:c r="E5" s="31"/>
+      <x:c r="F5" s="31"/>
+      <x:c r="G5" s="31"/>
       <x:c r="H5" s="32" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="I5" s="33" t="s"/>
+      <x:c r="I5" s="33"/>
     </x:row>
     <x:row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B7" s="35" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C7" s="35" t="s"/>
-      <x:c r="D7" s="35" t="s"/>
-      <x:c r="E7" s="35" t="s"/>
-      <x:c r="F7" s="35" t="s"/>
-      <x:c r="G7" s="35" t="s"/>
-      <x:c r="H7" s="35" t="s"/>
-      <x:c r="I7" s="35" t="s"/>
+      <x:c r="C7" s="35"/>
+      <x:c r="D7" s="35"/>
+      <x:c r="E7" s="35"/>
+      <x:c r="F7" s="35"/>
+      <x:c r="G7" s="35"/>
+      <x:c r="H7" s="35"/>
+      <x:c r="I7" s="35"/>
     </x:row>
     <x:row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B8" s="36" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C8" s="36" t="s"/>
-      <x:c r="D8" s="36" t="s"/>
-      <x:c r="E8" s="36" t="s"/>
-      <x:c r="F8" s="36" t="s"/>
-      <x:c r="G8" s="36" t="s"/>
-      <x:c r="H8" s="36" t="s"/>
-      <x:c r="I8" s="36" t="s"/>
+      <x:c r="C8" s="36"/>
+      <x:c r="D8" s="36"/>
+      <x:c r="E8" s="36"/>
+      <x:c r="F8" s="36"/>
+      <x:c r="G8" s="36"/>
+      <x:c r="H8" s="36"/>
+      <x:c r="I8" s="36"/>
     </x:row>
     <x:row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <x:c r="C10" s="6" t="s">
@@ -1105,78 +1114,78 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B11" s="7" t="s"/>
-      <x:c r="C11" s="8" t="s"/>
+      <x:c r="B11" s="7"/>
+      <x:c r="C11" s="8"/>
       <x:c r="D11" s="46" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E11" s="47" t="s"/>
-      <x:c r="F11" s="48" t="s"/>
+      <x:c r="E11" s="47"/>
+      <x:c r="F11" s="48"/>
       <x:c r="G11" s="46" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="H11" s="47" t="s"/>
-      <x:c r="I11" s="48" t="s"/>
+      <x:c r="H11" s="47"/>
+      <x:c r="I11" s="48"/>
     </x:row>
     <x:row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B12" s="49" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C12" s="50" t="s"/>
+      <x:c r="C12" s="50"/>
       <x:c r="D12" s="40">
         <x:f>"Admin"&amp;" "&amp;"root"</x:f>
       </x:c>
-      <x:c r="E12" s="41" t="s"/>
-      <x:c r="F12" s="42" t="s"/>
+      <x:c r="E12" s="41"/>
+      <x:c r="F12" s="42"/>
       <x:c r="G12" s="40">
-        <x:f>"Nguyễn Thị Lan"&amp;" "&amp;"Phương"</x:f>
-      </x:c>
-      <x:c r="H12" s="41" t="s"/>
-      <x:c r="I12" s="42" t="s"/>
+        <x:f>"Lê Văn"&amp;" "&amp;"Sâm"</x:f>
+      </x:c>
+      <x:c r="H12" s="41"/>
+      <x:c r="I12" s="42"/>
     </x:row>
     <x:row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B13" s="49" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C13" s="50" t="s"/>
-      <x:c r="D13" s="40" t="s"/>
-      <x:c r="E13" s="41" t="s"/>
-      <x:c r="F13" s="42" t="s"/>
+      <x:c r="C13" s="50"/>
+      <x:c r="D13" s="40"/>
+      <x:c r="E13" s="41"/>
+      <x:c r="F13" s="42"/>
       <x:c r="G13" s="40" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="H13" s="41" t="s"/>
-      <x:c r="I13" s="42" t="s"/>
+      <x:c r="H13" s="41"/>
+      <x:c r="I13" s="42"/>
     </x:row>
     <x:row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B14" s="49" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C14" s="50" t="s"/>
-      <x:c r="D14" s="40" t="s"/>
-      <x:c r="E14" s="41" t="s"/>
-      <x:c r="F14" s="42" t="s"/>
+      <x:c r="C14" s="50"/>
+      <x:c r="D14" s="40"/>
+      <x:c r="E14" s="41"/>
+      <x:c r="F14" s="42"/>
       <x:c r="G14" s="40" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="H14" s="41" t="s"/>
-      <x:c r="I14" s="42" t="s"/>
+      <x:c r="H14" s="41"/>
+      <x:c r="I14" s="42"/>
     </x:row>
     <x:row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B15" s="49" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C15" s="50" t="s"/>
+      <x:c r="C15" s="50"/>
       <x:c r="D15" s="40" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="E15" s="41" t="s"/>
-      <x:c r="F15" s="42" t="s"/>
+      <x:c r="E15" s="41"/>
+      <x:c r="F15" s="42"/>
       <x:c r="G15" s="40">
-        <x:f>""&amp;" / "&amp;""</x:f>
-      </x:c>
-      <x:c r="H15" s="41" t="s"/>
-      <x:c r="I15" s="42" t="s"/>
+        <x:f>"FA Department"&amp;" / "&amp;"Account"</x:f>
+      </x:c>
+      <x:c r="H15" s="41"/>
+      <x:c r="I15" s="42"/>
     </x:row>
     <x:row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <x:c r="B17" s="3" t="s">
@@ -1200,12 +1209,12 @@
       <x:c r="C21" s="51" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D21" s="51" t="s"/>
+      <x:c r="D21" s="51"/>
       <x:c r="E21" s="51" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="F21" s="51" t="s"/>
-      <x:c r="G21" s="51" t="s"/>
+      <x:c r="F21" s="51"/>
+      <x:c r="G21" s="51"/>
       <x:c r="H21" s="51" t="s">
         <x:v>25</x:v>
       </x:c>
@@ -1214,208 +1223,212 @@
       </x:c>
     </x:row>
     <x:row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="B22" s="13" t="s"/>
+      <x:c r="B22" s="13"/>
       <x:c r="C22" s="14" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D22" s="14" t="s"/>
+      <x:c r="D22" s="14"/>
       <x:c r="E22" s="14" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="F22" s="14" t="s"/>
-      <x:c r="G22" s="14" t="s"/>
-      <x:c r="H22" s="14" t="n">
+      <x:c r="F22" s="14"/>
+      <x:c r="G22" s="14"/>
+      <x:c r="H22" s="14">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="I22" s="14" t="s"/>
+      <x:c r="I22" s="14"/>
     </x:row>
     <x:row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="B23" s="13" t="s"/>
+      <x:c r="B23" s="13"/>
       <x:c r="C23" s="14" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="D23" s="14" t="s"/>
+      <x:c r="D23" s="14"/>
       <x:c r="E23" s="14" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="F23" s="14" t="s"/>
-      <x:c r="G23" s="14" t="s"/>
-      <x:c r="H23" s="14" t="n">
+      <x:c r="F23" s="14"/>
+      <x:c r="G23" s="14"/>
+      <x:c r="H23" s="14">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="I23" s="14" t="s"/>
-    </x:row>
-    <x:row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <x:c r="B24" s="13" t="s"/>
-      <x:c r="C24" s="20" t="s"/>
-      <x:c r="D24" s="21" t="s"/>
-      <x:c r="E24" s="22" t="s"/>
-      <x:c r="F24" s="23" t="s"/>
-      <x:c r="G24" s="24" t="s"/>
-      <x:c r="H24" s="14" t="s"/>
-      <x:c r="I24" s="14" t="s"/>
-    </x:row>
-    <x:row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <x:c r="B25" s="15" t="s"/>
-      <x:c r="C25" s="16" t="s"/>
-      <x:c r="D25" s="16" t="s"/>
-      <x:c r="E25" s="16" t="s"/>
-      <x:c r="F25" s="16" t="s"/>
-      <x:c r="G25" s="16" t="s"/>
-      <x:c r="H25" s="16" t="s"/>
-      <x:c r="I25" s="16" t="s"/>
+      <x:c r="I23" s="14"/>
+    </x:row>
+    <x:row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="B24" s="13"/>
+      <x:c r="C24" s="14" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D24" s="14"/>
+      <x:c r="E24" s="14" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F24" s="14"/>
+      <x:c r="G24" s="14"/>
+      <x:c r="H24" s="14">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I24" s="14"/>
+    </x:row>
+    <x:row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="B25" s="13"/>
+      <x:c r="C25" s="14" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D25" s="14"/>
+      <x:c r="E25" s="14" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F25" s="14"/>
+      <x:c r="G25" s="14"/>
+      <x:c r="H25" s="14">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I25" s="14"/>
+    </x:row>
+    <x:row r="26" spans="1:10">
+      <x:c r="B26" s="13"/>
+      <x:c r="C26" s="20"/>
+      <x:c r="D26" s="21"/>
+      <x:c r="E26" s="22"/>
+      <x:c r="F26" s="23"/>
+      <x:c r="G26" s="24"/>
+      <x:c r="H26" s="14"/>
+      <x:c r="I26" s="14"/>
     </x:row>
     <x:row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B27" s="1" t="s">
-        <x:v>31</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A28" s="10" t="s"/>
-      <x:c r="B28" s="19" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="E28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="F28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="H28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="I28" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="B27" s="15"/>
+      <x:c r="C27" s="16"/>
+      <x:c r="D27" s="16"/>
+      <x:c r="E27" s="16"/>
+      <x:c r="F27" s="16"/>
+      <x:c r="G27" s="16"/>
+      <x:c r="H27" s="16"/>
+      <x:c r="I27" s="16"/>
+    </x:row>
+    <x:row r="28" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="29" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A29" s="10" t="s"/>
-      <x:c r="B29" s="19" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C29" s="26" t="s"/>
-      <x:c r="D29" s="26" t="s"/>
-      <x:c r="E29" s="26" t="s"/>
-      <x:c r="F29" s="26" t="s"/>
-      <x:c r="G29" s="26" t="s"/>
-      <x:c r="H29" s="26" t="s"/>
-      <x:c r="I29" s="26" t="s"/>
+      <x:c r="B29" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
     </x:row>
     <x:row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A30" s="10" t="s"/>
+      <x:c r="A30" s="10"/>
       <x:c r="B30" s="19" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="C30" s="26" t="s"/>
-      <x:c r="D30" s="26" t="s"/>
-      <x:c r="E30" s="26" t="s"/>
-      <x:c r="F30" s="26" t="s"/>
-      <x:c r="G30" s="26" t="s"/>
-      <x:c r="H30" s="26" t="s"/>
-      <x:c r="I30" s="26" t="s"/>
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C30" s="19"/>
+      <x:c r="D30" s="19"/>
+      <x:c r="E30" s="19"/>
+      <x:c r="F30" s="19"/>
+      <x:c r="G30" s="19"/>
+      <x:c r="H30" s="19"/>
+      <x:c r="I30" s="19"/>
     </x:row>
     <x:row r="31" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A31" s="10" t="s"/>
+      <x:c r="A31" s="10"/>
       <x:c r="B31" s="19" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="C31" s="26" t="s"/>
-      <x:c r="D31" s="26" t="s"/>
-      <x:c r="E31" s="26" t="s"/>
-      <x:c r="F31" s="26" t="s"/>
-      <x:c r="G31" s="26" t="s"/>
-      <x:c r="H31" s="26" t="s"/>
-      <x:c r="I31" s="26" t="s"/>
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C31" s="26"/>
+      <x:c r="D31" s="26"/>
+      <x:c r="E31" s="26"/>
+      <x:c r="F31" s="26"/>
+      <x:c r="G31" s="26"/>
+      <x:c r="H31" s="26"/>
+      <x:c r="I31" s="26"/>
     </x:row>
     <x:row r="32" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="B32" s="28" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C32" s="29" t="s"/>
-      <x:c r="D32" s="29" t="s"/>
-      <x:c r="E32" s="29" t="s"/>
-      <x:c r="F32" s="29" t="s"/>
-      <x:c r="G32" s="29" t="s"/>
-      <x:c r="H32" s="29" t="s"/>
-      <x:c r="I32" s="29" t="s"/>
-    </x:row>
-    <x:row r="34" spans="1:10" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B34" s="26" t="s">
+      <x:c r="A32" s="10"/>
+      <x:c r="B32" s="19" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C34" s="26" t="s"/>
-      <x:c r="D34" s="26" t="s"/>
-      <x:c r="E34" s="26" t="s"/>
-      <x:c r="F34" s="26" t="s"/>
-      <x:c r="G34" s="26" t="s"/>
-      <x:c r="H34" s="26" t="s"/>
-      <x:c r="I34" s="26" t="s"/>
-    </x:row>
-    <x:row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <x:c r="B35" s="18" t="s">
+      <x:c r="C32" s="26"/>
+      <x:c r="D32" s="26"/>
+      <x:c r="E32" s="26"/>
+      <x:c r="F32" s="26"/>
+      <x:c r="G32" s="26"/>
+      <x:c r="H32" s="26"/>
+      <x:c r="I32" s="26"/>
+    </x:row>
+    <x:row r="33" spans="1:10">
+      <x:c r="A33" s="10"/>
+      <x:c r="B33" s="19" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C35" s="18" t="s"/>
-      <x:c r="D35" s="18" t="s"/>
-      <x:c r="E35" s="18" t="s"/>
-      <x:c r="F35" s="18" t="s"/>
-      <x:c r="G35" s="18" t="s"/>
-      <x:c r="H35" s="18" t="s"/>
-      <x:c r="I35" s="18" t="s"/>
+      <x:c r="C33" s="26"/>
+      <x:c r="D33" s="26"/>
+      <x:c r="E33" s="26"/>
+      <x:c r="F33" s="26"/>
+      <x:c r="G33" s="26"/>
+      <x:c r="H33" s="26"/>
+      <x:c r="I33" s="26"/>
+    </x:row>
+    <x:row r="34" spans="1:10" ht="33" customHeight="1" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="B34" s="28" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C34" s="29"/>
+      <x:c r="D34" s="29"/>
+      <x:c r="E34" s="29"/>
+      <x:c r="F34" s="29"/>
+      <x:c r="G34" s="29"/>
+      <x:c r="H34" s="29"/>
+      <x:c r="I34" s="29"/>
     </x:row>
     <x:row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B36" s="17" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C36" s="17" t="s"/>
-      <x:c r="D36" s="17" t="s"/>
-      <x:c r="E36" s="1" t="s"/>
-      <x:c r="F36" s="17" t="s">
+      <x:c r="B36" s="26" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="G36" s="17" t="s"/>
-      <x:c r="H36" s="17" t="s"/>
-      <x:c r="I36" s="1" t="s"/>
-    </x:row>
-    <x:row r="37" spans="1:10" s="0" customFormat="1">
-      <x:c r="A37" s="0" t="s"/>
-      <x:c r="B37" s="0" t="s"/>
-      <x:c r="C37" s="0" t="s"/>
-      <x:c r="D37" s="0" t="s"/>
-      <x:c r="E37" s="0" t="s"/>
-      <x:c r="F37" s="0" t="s"/>
-      <x:c r="G37" s="0" t="s"/>
-      <x:c r="H37" s="0" t="s"/>
-      <x:c r="I37" s="0" t="s"/>
-      <x:c r="J37" s="0" t="s"/>
-    </x:row>
-    <x:row r="40" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A40" s="0" t="s"/>
-      <x:c r="B40" s="17">
+      <x:c r="C36" s="26"/>
+      <x:c r="D36" s="26"/>
+      <x:c r="E36" s="26"/>
+      <x:c r="F36" s="26"/>
+      <x:c r="G36" s="26"/>
+      <x:c r="H36" s="26"/>
+      <x:c r="I36" s="26"/>
+    </x:row>
+    <x:row r="37" spans="1:10">
+      <x:c r="B37" s="18" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C37" s="18"/>
+      <x:c r="D37" s="18"/>
+      <x:c r="E37" s="18"/>
+      <x:c r="F37" s="18"/>
+      <x:c r="G37" s="18"/>
+      <x:c r="H37" s="18"/>
+      <x:c r="I37" s="18"/>
+    </x:row>
+    <x:row r="38" spans="1:10">
+      <x:c r="B38" s="17" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C38" s="17"/>
+      <x:c r="D38" s="17"/>
+      <x:c r="E38" s="1"/>
+      <x:c r="F38" s="17" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G38" s="17"/>
+      <x:c r="H38" s="17"/>
+      <x:c r="I38" s="1"/>
+    </x:row>
+    <x:row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <x:row r="42" spans="1:10">
+      <x:c r="B42" s="17">
         <x:f>"Admin"&amp;" "&amp;"root"</x:f>
       </x:c>
-      <x:c r="C40" s="17" t="s"/>
-      <x:c r="D40" s="17" t="s"/>
-      <x:c r="E40" s="0" t="s"/>
-      <x:c r="F40" s="17">
-        <x:f>"Nguyễn Thị Lan"&amp;" "&amp;"Phương"</x:f>
-      </x:c>
-      <x:c r="G40" s="17" t="s"/>
-      <x:c r="H40" s="17" t="s"/>
-      <x:c r="I40" s="0" t="s"/>
-      <x:c r="J40" s="0" t="s"/>
+      <x:c r="C42" s="17"/>
+      <x:c r="D42" s="17"/>
+      <x:c r="F42" s="17">
+        <x:f>"Lê Văn"&amp;" "&amp;"Sâm"</x:f>
+      </x:c>
+      <x:c r="G42" s="17"/>
+      <x:c r="H42" s="17"/>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="40">
+  <x:mergeCells count="44">
     <x:mergeCell ref="B5:C5"/>
     <x:mergeCell ref="D5:G5"/>
     <x:mergeCell ref="H5:I5"/>
@@ -1445,17 +1458,21 @@
     <x:mergeCell ref="E24:G24"/>
     <x:mergeCell ref="C25:D25"/>
     <x:mergeCell ref="E25:G25"/>
-    <x:mergeCell ref="B28:I28"/>
-    <x:mergeCell ref="B29:I29"/>
+    <x:mergeCell ref="C26:D26"/>
+    <x:mergeCell ref="E26:G26"/>
+    <x:mergeCell ref="C27:D27"/>
+    <x:mergeCell ref="E27:G27"/>
     <x:mergeCell ref="B30:I30"/>
     <x:mergeCell ref="B31:I31"/>
     <x:mergeCell ref="B32:I32"/>
+    <x:mergeCell ref="B33:I33"/>
     <x:mergeCell ref="B34:I34"/>
-    <x:mergeCell ref="B35:I35"/>
-    <x:mergeCell ref="B36:D36"/>
-    <x:mergeCell ref="F36:H36"/>
-    <x:mergeCell ref="B40:D40"/>
-    <x:mergeCell ref="F40:H40"/>
+    <x:mergeCell ref="B36:I36"/>
+    <x:mergeCell ref="B37:I37"/>
+    <x:mergeCell ref="B38:D38"/>
+    <x:mergeCell ref="F38:H38"/>
+    <x:mergeCell ref="B42:D42"/>
+    <x:mergeCell ref="F42:H42"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.5" right="0.25" top="0.5" bottom="0.5" header="0" footer="0.05"/>

</xml_diff>